<commit_message>
More custom layout: sheet name
</commit_message>
<xml_diff>
--- a/docs/Examples/CustomLayout/custom-layout.xlsx
+++ b/docs/Examples/CustomLayout/custom-layout.xlsx
@@ -8,11 +8,11 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="KNX Group Addresses" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="KNX GAs" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Room Book" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'KNX Group Addresses'!$B$3:$I$273</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'KNX GAs'!$B$3:$I$273</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Room Book'!$A$8:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">'Room Book'!$B$8:$I$11</definedName>
   </definedNames>
@@ -678,7 +678,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1033,7 +1033,7 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="3" s="6" customFormat="true" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
@@ -1063,8 +1063,8 @@
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>

</xml_diff>